<commit_message>
Sync local over remote
</commit_message>
<xml_diff>
--- a/data/basedatos.xlsx
+++ b/data/basedatos.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61B4738-8451-4E48-AEB1-4D39990B9250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D94B7D-7DC4-438D-8927-82AE6A002CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="709" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MUEBLESFRIOS" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="SIEMENS" sheetId="11" r:id="rId9"/>
     <sheet name="MURRELEKTRONIK" sheetId="9" r:id="rId10"/>
     <sheet name="OPCIONES CO2" sheetId="6" r:id="rId11"/>
-    <sheet name="CABLE POTENCIA" sheetId="12" r:id="rId12"/>
+    <sheet name="PUENTES" sheetId="13" r:id="rId12"/>
+    <sheet name="CABLE POTENCIA" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4255" uniqueCount="1057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4364" uniqueCount="1084">
   <si>
     <t>AUTOSERVICIO AQUILA</t>
   </si>
@@ -12533,9 +12534,6 @@
     <t>(MARCA DE ELEMENTOS:A(B)D(2)K(1)J("UL")=B,C,F,G,H,I,L)*#</t>
   </si>
   <si>
-    <t>(MARCA DE ELEMENTOS:A(B)D(20)K(3)J("UL")=B,C,F,G,H,I,L)*#</t>
-  </si>
-  <si>
     <t>P1-#F1</t>
   </si>
   <si>
@@ -13017,6 +13015,90 @@
   </si>
   <si>
     <t>MARCA DE ELEMENTOS:A(CA)N(8)=B,C,F,G,H,I,L</t>
+  </si>
+  <si>
+    <t>MARCA</t>
+  </si>
+  <si>
+    <t>FAMILIA</t>
+  </si>
+  <si>
+    <t>BEA38-4</t>
+  </si>
+  <si>
+    <t>PUENTES</t>
+  </si>
+  <si>
+    <t>CODIGO PUENTES</t>
+  </si>
+  <si>
+    <t>BEA65-4</t>
+  </si>
+  <si>
+    <t>(MARCA DE ELEMENTOS:A(B)D(32)K(3)J("UL")=B,C,F,G,H,I,L)*#</t>
+  </si>
+  <si>
+    <t>SISTEMA RILINE RITTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SV RILINE60 SOPORTE DE BARRAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SV RILINE60 BANDEJA BASE SECCION </t>
+  </si>
+  <si>
+    <t>SV RILINE60 CUBIERTA FINA 9340070</t>
+  </si>
+  <si>
+    <t>SV ADAPTADOR CONEX 800A-690 9342280</t>
+  </si>
+  <si>
+    <t>SVSB</t>
+  </si>
+  <si>
+    <t>SVBB</t>
+  </si>
+  <si>
+    <t>SVCF</t>
+  </si>
+  <si>
+    <t>SVFC</t>
+  </si>
+  <si>
+    <t>BARRA COBRE P/TAB BARRA NAL001 30X10XMTR</t>
+  </si>
+  <si>
+    <t>SVBC</t>
+  </si>
+  <si>
+    <t>BARRA COBRE  30X10</t>
+  </si>
+  <si>
+    <t>GIRO PARA BARRAJE 800A</t>
+  </si>
+  <si>
+    <t>PAPAS PARA FINAL DE BARRAJE</t>
+  </si>
+  <si>
+    <t>BANDEJA BASE PARA RILINE</t>
+  </si>
+  <si>
+    <t>SEPARADORES DE BARRAS</t>
+  </si>
+  <si>
+    <t>MARCA DE ELEMENTOS:A(SVSB)J("UL")=B,C,F,G,H,I,L</t>
+  </si>
+  <si>
+    <t>MARCA DE ELEMENTOS:A(SVFC)J("UL")=B,C,F,G,H,I,L</t>
+  </si>
+  <si>
+    <t>MARCA DE ELEMENTOS:A(SVBB)=B,C,F,G,H,I,L</t>
+  </si>
+  <si>
+    <t>MARCA DE ELEMENTOS:A(SVCF)=B,C,F,G,H,I,L</t>
+  </si>
+  <si>
+    <t>MARCA DE ELEMENTOS:A(SVBC)=B,C,F,G,H,I,L</t>
   </si>
 </sst>
 </file>
@@ -17617,10 +17699,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41762CEE-4DE1-4DF6-BCA1-F4F1B5362F1B}">
-  <dimension ref="A1:BH108"/>
+  <dimension ref="A1:BH119"/>
   <sheetViews>
-    <sheetView topLeftCell="AV10" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="BH25" sqref="BH25"/>
+    <sheetView tabSelected="1" topLeftCell="AA97" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="AC114" sqref="AC114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17682,13 +17764,13 @@
         <v>662</v>
       </c>
       <c r="W1" s="55" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="X1" s="56" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="Y1" s="56" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="Z1" s="56" t="s">
         <v>760</v>
@@ -17721,13 +17803,13 @@
         <v>44</v>
       </c>
       <c r="AX1" s="58" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="AY1" s="51" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="AZ1" s="59" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="BA1" s="59" t="s">
         <v>761</v>
@@ -17848,7 +17930,7 @@
         <v>780</v>
       </c>
       <c r="BE3" s="49" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="BF3" s="49"/>
       <c r="BG3" s="30"/>
@@ -18423,10 +18505,10 @@
       <c r="BB13" s="30"/>
       <c r="BC13" s="30"/>
       <c r="BD13" s="30" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BE13" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="BF13" s="30" t="s">
         <v>801</v>
@@ -19093,7 +19175,7 @@
       <c r="X27" s="30"/>
       <c r="Y27" s="30"/>
       <c r="Z27" s="30" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="AA27" s="30"/>
       <c r="AB27" s="30" t="s">
@@ -19149,7 +19231,7 @@
         <v>704</v>
       </c>
       <c r="AA28" s="53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="AB28" s="30" t="s">
         <v>705</v>
@@ -19294,10 +19376,10 @@
       <c r="BB30" s="30"/>
       <c r="BC30" s="30"/>
       <c r="BD30" s="30" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="BE30" s="30" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="BF30" s="30" t="s">
         <v>801</v>
@@ -19329,20 +19411,20 @@
         <v>1</v>
       </c>
       <c r="Z31" s="30" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="AA31" s="30"/>
       <c r="AB31" s="42" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AC31" s="42" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AD31" s="30" t="s">
         <v>652</v>
       </c>
       <c r="AE31" s="30" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="AF31" s="30" t="s">
         <v>763</v>
@@ -19359,10 +19441,10 @@
       <c r="BB31" s="30"/>
       <c r="BC31" s="30"/>
       <c r="BD31" s="30" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="BE31" s="30" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="BF31" s="30" t="s">
         <v>801</v>
@@ -19392,7 +19474,7 @@
         <v>1</v>
       </c>
       <c r="Z32" s="30" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="AA32" s="30"/>
       <c r="AB32" s="30"/>
@@ -19414,10 +19496,10 @@
       </c>
       <c r="BC32" s="30"/>
       <c r="BD32" s="30" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="BE32" s="30" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="BF32" s="30"/>
       <c r="BG32" s="30"/>
@@ -19441,7 +19523,7 @@
         <v>1</v>
       </c>
       <c r="Z33" s="30" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AA33" s="30"/>
       <c r="AB33" s="30"/>
@@ -19469,10 +19551,10 @@
       </c>
       <c r="BC33" s="30"/>
       <c r="BD33" s="30" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="BE33" s="30" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="BF33" s="30"/>
       <c r="BG33" s="30"/>
@@ -19494,7 +19576,7 @@
       <c r="X34" s="30"/>
       <c r="Y34" s="30"/>
       <c r="Z34" s="30" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AA34" s="30"/>
       <c r="AB34" s="30"/>
@@ -19522,10 +19604,10 @@
       </c>
       <c r="BC34" s="30"/>
       <c r="BD34" s="30" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="BE34" s="30" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="BF34" s="30"/>
       <c r="BG34" s="30"/>
@@ -19547,7 +19629,7 @@
       <c r="X35" s="30"/>
       <c r="Y35" s="30"/>
       <c r="Z35" s="30" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AA35" s="30"/>
       <c r="AB35" s="30"/>
@@ -19575,10 +19657,10 @@
       </c>
       <c r="BC35" s="30"/>
       <c r="BD35" s="30" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="BE35" s="30" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="BF35" s="30"/>
       <c r="BG35" s="30"/>
@@ -19600,7 +19682,7 @@
       <c r="X36" s="30"/>
       <c r="Y36" s="30"/>
       <c r="Z36" s="30" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="AA36" s="30"/>
       <c r="AB36" s="30"/>
@@ -19628,10 +19710,10 @@
       </c>
       <c r="BC36" s="30"/>
       <c r="BD36" s="30" t="s">
+        <v>1054</v>
+      </c>
+      <c r="BE36" s="30" t="s">
         <v>1055</v>
-      </c>
-      <c r="BE36" s="30" t="s">
-        <v>1056</v>
       </c>
       <c r="BF36" s="30"/>
       <c r="BG36" s="30"/>
@@ -19647,7 +19729,7 @@
       <c r="X37" s="30"/>
       <c r="Y37" s="30"/>
       <c r="Z37" s="30" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="AA37" s="30"/>
       <c r="AB37" s="30"/>
@@ -19675,10 +19757,10 @@
       </c>
       <c r="BC37" s="30"/>
       <c r="BD37" s="30" t="s">
+        <v>1054</v>
+      </c>
+      <c r="BE37" s="30" t="s">
         <v>1055</v>
-      </c>
-      <c r="BE37" s="30" t="s">
-        <v>1056</v>
       </c>
       <c r="BF37" s="30"/>
       <c r="BG37" s="30"/>
@@ -19932,20 +20014,20 @@
         <v>1</v>
       </c>
       <c r="Z44" s="30" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="AA44" s="30"/>
       <c r="AB44" s="42" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="AC44" s="42" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AD44" s="30" t="s">
         <v>652</v>
       </c>
       <c r="AE44" s="30" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="AF44" s="30" t="s">
         <v>763</v>
@@ -19981,7 +20063,7 @@
       <c r="X45" s="30"/>
       <c r="Y45" s="30"/>
       <c r="Z45" s="30" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="AA45" s="30"/>
       <c r="AB45" s="30"/>
@@ -20028,7 +20110,7 @@
       <c r="X46" s="30"/>
       <c r="Y46" s="30"/>
       <c r="Z46" s="30" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="AA46" s="30"/>
       <c r="AB46" s="30"/>
@@ -20087,7 +20169,7 @@
       <c r="X47" s="30"/>
       <c r="Y47" s="30"/>
       <c r="Z47" s="30" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="AA47" s="30"/>
       <c r="AB47" s="30"/>
@@ -20140,7 +20222,7 @@
       <c r="X48" s="30"/>
       <c r="Y48" s="30"/>
       <c r="Z48" s="30" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="AA48" s="30"/>
       <c r="AB48" s="30"/>
@@ -20193,7 +20275,7 @@
       <c r="X49" s="30"/>
       <c r="Y49" s="30"/>
       <c r="Z49" s="30" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="AA49" s="30"/>
       <c r="AB49" s="30"/>
@@ -20583,10 +20665,10 @@
       <c r="BB55" s="46"/>
       <c r="BC55" s="46"/>
       <c r="BD55" s="30" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="BE55" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="BF55" s="30" t="s">
         <v>801</v>
@@ -20614,7 +20696,7 @@
       <c r="X56" s="30"/>
       <c r="Y56" s="30"/>
       <c r="Z56" s="30" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="AA56" s="30"/>
       <c r="AB56" s="30"/>
@@ -20678,7 +20760,7 @@
       <c r="X58" s="30"/>
       <c r="Y58" s="30"/>
       <c r="Z58" s="30" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="AA58" s="30"/>
       <c r="AB58" s="30"/>
@@ -20806,14 +20888,14 @@
       <c r="X62" s="30"/>
       <c r="Y62" s="30"/>
       <c r="Z62" s="30" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="AA62" s="30"/>
       <c r="AB62" s="30" t="s">
         <v>892</v>
       </c>
       <c r="AC62" s="30" t="s">
-        <v>895</v>
+        <v>1062</v>
       </c>
       <c r="AD62" s="30" t="s">
         <v>892</v>
@@ -20892,7 +20974,7 @@
       <c r="X64" s="30"/>
       <c r="Y64" s="30"/>
       <c r="Z64" s="30" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="AA64" s="30"/>
       <c r="AB64" s="30"/>
@@ -20914,7 +20996,7 @@
       <c r="X65" s="30"/>
       <c r="Y65" s="30"/>
       <c r="Z65" s="30" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="AA65" s="30"/>
       <c r="AB65" s="30"/>
@@ -20944,7 +21026,7 @@
         <v>1</v>
       </c>
       <c r="Z66" s="30" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="AA66" s="30"/>
       <c r="AB66" s="30"/>
@@ -20972,7 +21054,7 @@
       <c r="X67" s="30"/>
       <c r="Y67" s="30"/>
       <c r="Z67" s="30" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="AA67" s="30"/>
       <c r="AB67" s="30"/>
@@ -21000,7 +21082,7 @@
       <c r="X68" s="30"/>
       <c r="Y68" s="30"/>
       <c r="Z68" s="30" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="AA68" s="30"/>
       <c r="AB68" s="30"/>
@@ -21030,7 +21112,7 @@
         <v>1</v>
       </c>
       <c r="Z69" s="30" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AA69" s="30"/>
       <c r="AB69" s="30"/>
@@ -21058,7 +21140,7 @@
       <c r="X70" s="30"/>
       <c r="Y70" s="30"/>
       <c r="Z70" s="30" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="AA70" s="30"/>
       <c r="AB70" s="30"/>
@@ -21086,7 +21168,7 @@
       <c r="X71" s="30"/>
       <c r="Y71" s="30"/>
       <c r="Z71" s="30" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="AA71" s="30"/>
       <c r="AB71" s="30"/>
@@ -21120,7 +21202,7 @@
       <c r="X72" s="30"/>
       <c r="Y72" s="30"/>
       <c r="Z72" s="30" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="AA72" s="30"/>
       <c r="AB72" s="30"/>
@@ -21148,7 +21230,7 @@
       <c r="X73" s="30"/>
       <c r="Y73" s="30"/>
       <c r="Z73" s="30" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="AA73" s="30"/>
       <c r="AB73" s="30"/>
@@ -21355,9 +21437,15 @@
       <c r="AI79" s="44"/>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A80" s="43"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="44"/>
+      <c r="A80" s="43" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B80" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="C80" s="44" t="s">
+        <v>44</v>
+      </c>
       <c r="W80" s="43"/>
       <c r="X80" s="30">
         <v>1</v>
@@ -21426,11 +21514,11 @@
       <c r="X82" s="30"/>
       <c r="Y82" s="30"/>
       <c r="Z82" s="30" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="AA82" s="30"/>
       <c r="AB82" s="30" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="AC82" s="30" t="s">
         <v>860</v>
@@ -21456,20 +21544,20 @@
       <c r="X83" s="30"/>
       <c r="Y83" s="30"/>
       <c r="Z83" s="30" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="AA83" s="30"/>
       <c r="AB83" s="30" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="AC83" s="30" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AD83" s="30" t="s">
         <v>652</v>
       </c>
       <c r="AE83" s="30" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="AF83" s="30" t="s">
         <v>763</v>
@@ -21486,11 +21574,11 @@
       <c r="X84" s="30"/>
       <c r="Y84" s="30"/>
       <c r="Z84" s="30" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="AA84" s="30"/>
       <c r="AB84" s="30" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="AC84" t="s">
         <v>795</v>
@@ -21516,14 +21604,14 @@
       <c r="X85" s="30"/>
       <c r="Y85" s="30"/>
       <c r="Z85" s="30" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="AA85" s="30"/>
       <c r="AB85" s="30" t="s">
+        <v>960</v>
+      </c>
+      <c r="AC85" s="30" t="s">
         <v>961</v>
-      </c>
-      <c r="AC85" s="30" t="s">
-        <v>962</v>
       </c>
       <c r="AD85" s="30" t="s">
         <v>652</v>
@@ -21546,14 +21634,14 @@
       <c r="X86" s="30"/>
       <c r="Y86" s="30"/>
       <c r="Z86" s="30" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="AA86" s="30"/>
       <c r="AB86" s="30" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="AC86" s="30" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AD86" s="30" t="s">
         <v>652</v>
@@ -21576,14 +21664,14 @@
       <c r="X87" s="30"/>
       <c r="Y87" s="30"/>
       <c r="Z87" s="30" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="AA87" s="30"/>
       <c r="AB87" s="30" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="AC87" s="30" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AD87" s="30" t="s">
         <v>652</v>
@@ -21606,14 +21694,14 @@
       <c r="X88" s="30"/>
       <c r="Y88" s="30"/>
       <c r="Z88" s="30" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="AA88" s="30"/>
       <c r="AB88" s="30" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="AC88" s="30" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AD88" s="30" t="s">
         <v>652</v>
@@ -21636,14 +21724,14 @@
       <c r="X89" s="30"/>
       <c r="Y89" s="30"/>
       <c r="Z89" s="30" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="AA89" s="30"/>
       <c r="AB89" s="30" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="AC89" s="30" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AD89" s="30" t="s">
         <v>652</v>
@@ -21666,14 +21754,14 @@
       <c r="X90" s="30"/>
       <c r="Y90" s="30"/>
       <c r="Z90" s="30" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="AA90" s="30"/>
       <c r="AB90" s="30" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="AC90" s="30" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AD90" s="30" t="s">
         <v>652</v>
@@ -21696,14 +21784,14 @@
       <c r="X91" s="30"/>
       <c r="Y91" s="30"/>
       <c r="Z91" s="30" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="AA91" s="30"/>
       <c r="AB91" s="30" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="AC91" s="30" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="AD91" s="30" t="s">
         <v>652</v>
@@ -21726,20 +21814,20 @@
       <c r="X92" s="30"/>
       <c r="Y92" s="30"/>
       <c r="Z92" s="30" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="AA92" s="30"/>
       <c r="AB92" s="30" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="AC92" s="30" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AD92" s="30" t="s">
         <v>652</v>
       </c>
       <c r="AE92" s="30" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="AF92" s="30" t="s">
         <v>763</v>
@@ -21756,20 +21844,20 @@
       <c r="X93" s="30"/>
       <c r="Y93" s="30"/>
       <c r="Z93" s="30" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="AA93" s="30"/>
       <c r="AB93" s="30" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="AC93" s="30" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AD93" s="30" t="s">
         <v>652</v>
       </c>
       <c r="AE93" s="30" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="AF93" s="30" t="s">
         <v>763</v>
@@ -21786,11 +21874,11 @@
       <c r="X94" s="30"/>
       <c r="Y94" s="30"/>
       <c r="Z94" s="30" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="AA94" s="30"/>
       <c r="AB94" s="30" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="AC94" s="30" t="s">
         <v>826</v>
@@ -21816,11 +21904,11 @@
       <c r="X95" s="30"/>
       <c r="Y95" s="30"/>
       <c r="Z95" s="30" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="AA95" s="30"/>
       <c r="AB95" s="30" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="AC95" s="30" t="s">
         <v>806</v>
@@ -21846,11 +21934,11 @@
       <c r="X96" s="30"/>
       <c r="Y96" s="30"/>
       <c r="Z96" s="30" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="AA96" s="30"/>
       <c r="AB96" s="30" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="AC96" s="30" t="s">
         <v>806</v>
@@ -22167,10 +22255,10 @@
       <c r="Z108" s="46"/>
       <c r="AA108" s="46"/>
       <c r="AB108" s="46" t="s">
+        <v>926</v>
+      </c>
+      <c r="AC108" s="46" t="s">
         <v>927</v>
-      </c>
-      <c r="AC108" s="46" t="s">
-        <v>928</v>
       </c>
       <c r="AD108" s="46" t="s">
         <v>647</v>
@@ -22184,6 +22272,106 @@
       <c r="AG108" s="46"/>
       <c r="AH108" s="46"/>
       <c r="AI108" s="47"/>
+    </row>
+    <row r="109" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AB109" s="30" t="s">
+        <v>1064</v>
+      </c>
+      <c r="AC109" s="30" t="s">
+        <v>1079</v>
+      </c>
+      <c r="AD109" s="43" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AE109" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="AF109" s="30" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="110" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AB110" s="30" t="s">
+        <v>1065</v>
+      </c>
+      <c r="AC110" s="30" t="s">
+        <v>1081</v>
+      </c>
+      <c r="AD110" s="43" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AE110" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="AF110" s="30" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="111" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AB111" s="30" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AC111" s="30" t="s">
+        <v>1082</v>
+      </c>
+      <c r="AD111" s="43" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AE111" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="AF111" s="30" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="112" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AB112" s="30" t="s">
+        <v>1067</v>
+      </c>
+      <c r="AC112" s="30" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AD112" s="43" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AE112" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="AF112" s="30" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="113" spans="28:32" x14ac:dyDescent="0.3">
+      <c r="AB113" s="33" t="s">
+        <v>1072</v>
+      </c>
+      <c r="AC113" s="30" t="s">
+        <v>1083</v>
+      </c>
+      <c r="AD113" s="43" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AE113" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="AF113" s="30" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="115" spans="28:32" x14ac:dyDescent="0.3">
+      <c r="AC115" s="33"/>
+    </row>
+    <row r="116" spans="28:32" x14ac:dyDescent="0.3">
+      <c r="AC116" s="33"/>
+    </row>
+    <row r="117" spans="28:32" x14ac:dyDescent="0.3">
+      <c r="AC117" s="33"/>
+    </row>
+    <row r="118" spans="28:32" x14ac:dyDescent="0.3">
+      <c r="AC118" s="33"/>
+    </row>
+    <row r="119" spans="28:32" x14ac:dyDescent="0.3">
+      <c r="AC119" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22191,6 +22379,257 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43B5C33-03F8-4C10-985E-293D89572975}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1" t="s">
+        <v>801</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>484</v>
+      </c>
+      <c r="G2" s="33">
+        <v>134099</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="J2" s="38">
+        <v>130500</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>498</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>494</v>
+      </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30" t="s">
+        <v>454</v>
+      </c>
+      <c r="J3" s="38">
+        <v>130507</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>509</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>504</v>
+      </c>
+      <c r="G4" s="33">
+        <v>134188</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J4" s="38">
+        <v>130189</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>517</v>
+      </c>
+      <c r="G5" s="33">
+        <v>134180</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="J5" s="38">
+        <v>130194</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>525</v>
+      </c>
+      <c r="G6" s="33">
+        <v>134181</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="J6" s="38">
+        <v>130501</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G7" s="33">
+        <v>134098</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>498</v>
+      </c>
+      <c r="J7" s="38">
+        <v>130188</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G8" s="33">
+        <v>134182</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>509</v>
+      </c>
+      <c r="J8" s="38">
+        <v>130502</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G9" s="33">
+        <v>134183</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>517</v>
+      </c>
+      <c r="J9" s="38">
+        <v>130192</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G10" s="30"/>
+      <c r="H10" s="30" t="s">
+        <v>525</v>
+      </c>
+      <c r="J10" s="38">
+        <v>130503</v>
+      </c>
+      <c r="K10" s="33" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G11" s="33">
+        <v>134094</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>535</v>
+      </c>
+      <c r="J11" s="38">
+        <v>130193</v>
+      </c>
+      <c r="K11" s="33" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G12" s="33">
+        <v>134095</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>545</v>
+      </c>
+      <c r="J12" s="38">
+        <v>130505</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G13" s="33">
+        <v>134184</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G14" s="30"/>
+      <c r="H14" s="30" t="s">
+        <v>561</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FCBEE1-8496-4AB8-ADAC-958BF7083BCD}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -22207,7 +22646,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="91" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
@@ -22215,24 +22654,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="67" t="s">
+        <v>983</v>
+      </c>
+      <c r="B2" s="68" t="s">
         <v>984</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="C2" s="68" t="s">
         <v>985</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="D2" s="69" t="s">
         <v>986</v>
-      </c>
-      <c r="D2" s="69" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C3" s="30">
         <v>20</v>
@@ -22243,10 +22682,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C4" s="30">
         <v>30</v>
@@ -22257,10 +22696,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C5" s="30">
         <v>40</v>
@@ -22271,10 +22710,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="43" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C6" s="30">
         <v>55</v>
@@ -22285,10 +22724,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C7" s="30">
         <v>70</v>
@@ -22299,10 +22738,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C8" s="30">
         <v>95</v>
@@ -22316,10 +22755,10 @@
         <v>358</v>
       </c>
       <c r="B9" s="30" t="s">
+        <v>993</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>994</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>995</v>
       </c>
       <c r="D9" s="44">
         <v>150</v>
@@ -22330,10 +22769,10 @@
         <v>359</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D10" s="44">
         <v>175</v>
@@ -22344,10 +22783,10 @@
         <v>361</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D11" s="44">
         <v>200</v>
@@ -22358,10 +22797,10 @@
         <v>363</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D12" s="44">
         <v>230</v>
@@ -22369,13 +22808,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="43" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B13" s="30">
         <v>127</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D13" s="44">
         <v>255</v>
@@ -22383,13 +22822,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="43" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B14" s="30">
         <v>152</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D14" s="44">
         <v>285</v>
@@ -22397,13 +22836,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="43" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B15" s="30">
         <v>177</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D15" s="44">
         <v>310</v>
@@ -22411,13 +22850,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="43" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B16" s="30">
         <v>203</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D16" s="44">
         <v>335</v>
@@ -22425,13 +22864,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B17" s="30">
         <v>253</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D17" s="44">
         <v>380</v>
@@ -22439,13 +22878,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B18" s="30">
         <v>304</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D18" s="44">
         <v>420</v>
@@ -22453,13 +22892,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="43" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B19" s="30">
         <v>355</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D19" s="44">
         <v>460</v>
@@ -22467,13 +22906,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B20" s="30">
         <v>380</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D20" s="44">
         <v>475</v>
@@ -22481,13 +22920,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="43" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B21" s="30">
         <v>405</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D21" s="44">
         <v>490</v>
@@ -22495,13 +22934,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B22" s="30">
         <v>456</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D22" s="44">
         <v>520</v>
@@ -22509,13 +22948,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B23" s="30">
         <v>506</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D23" s="44">
         <v>545</v>
@@ -22523,13 +22962,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="43" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B24" s="30">
         <v>633</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D24" s="44">
         <v>590</v>
@@ -22537,13 +22976,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="43" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B25" s="30">
         <v>760</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D25" s="44">
         <v>625</v>
@@ -22551,13 +22990,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="43" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B26" s="30">
         <v>887</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D26" s="44">
         <v>650</v>
@@ -22565,13 +23004,13 @@
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="45" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B27" s="46">
         <v>1013</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D27" s="47">
         <v>665</v>
@@ -25693,10 +26132,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F54C4A5-BAB8-4C9F-811A-677C90088FCD}">
-  <dimension ref="A1:S83"/>
+  <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N79" sqref="N79"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="10200" topLeftCell="O1"/>
+      <selection activeCell="A24" sqref="A24"/>
+      <selection pane="topRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25712,11 +26153,13 @@
     <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>604</v>
       </c>
@@ -25765,8 +26208,14 @@
       <c r="P1" s="35" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q1" s="35" t="s">
+        <v>1059</v>
+      </c>
+      <c r="R1" s="35" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>597</v>
       </c>
@@ -25803,8 +26252,10 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q2" s="30"/>
+      <c r="R2" s="33"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>597</v>
       </c>
@@ -25839,8 +26290,10 @@
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
       <c r="P3" s="30"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q3" s="30"/>
+      <c r="R3" s="33"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>597</v>
       </c>
@@ -25848,7 +26301,7 @@
         <v>134188</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D4" s="30">
         <v>4</v>
@@ -25877,8 +26330,10 @@
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q4" s="30"/>
+      <c r="R4" s="33"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>597</v>
       </c>
@@ -25915,8 +26370,10 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q5" s="30"/>
+      <c r="R5" s="33"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>597</v>
       </c>
@@ -25953,8 +26410,14 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q6" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R6" s="33">
+        <v>130511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>597</v>
       </c>
@@ -25991,17 +26454,23 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
       <c r="P7" s="30"/>
-      <c r="Q7" t="s">
+      <c r="Q7" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R7" s="33">
+        <v>130511</v>
+      </c>
+      <c r="S7" t="s">
         <v>597</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>427</v>
       </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>597</v>
       </c>
@@ -26038,14 +26507,20 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
       <c r="P8" s="30"/>
-      <c r="Q8" t="s">
+      <c r="Q8" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R8" s="33">
+        <v>130511</v>
+      </c>
+      <c r="S8" t="s">
         <v>605</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>597</v>
       </c>
@@ -26082,14 +26557,20 @@
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
       <c r="P9" s="30"/>
-      <c r="Q9" t="s">
+      <c r="Q9" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R9" s="33">
+        <v>130511</v>
+      </c>
+      <c r="S9" t="s">
         <v>598</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
         <v>597</v>
       </c>
@@ -26124,17 +26605,23 @@
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
       <c r="P10" s="30"/>
-      <c r="Q10" t="s">
+      <c r="Q10" s="30" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R10" s="33">
+        <v>130510</v>
+      </c>
+      <c r="S10" t="s">
         <v>599</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>428</v>
       </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>597</v>
       </c>
@@ -26171,14 +26658,20 @@
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
       <c r="P11" s="30"/>
-      <c r="Q11" t="s">
+      <c r="Q11" s="30" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R11" s="33">
+        <v>130510</v>
+      </c>
+      <c r="S11" t="s">
         <v>600</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>597</v>
       </c>
@@ -26215,14 +26708,20 @@
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
       <c r="P12" s="30"/>
-      <c r="Q12" t="s">
+      <c r="Q12" s="30" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R12" s="33">
+        <v>130510</v>
+      </c>
+      <c r="S12" t="s">
         <v>601</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
         <v>597</v>
       </c>
@@ -26259,17 +26758,23 @@
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
       <c r="P13" s="30"/>
-      <c r="Q13" t="s">
+      <c r="Q13" s="30" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R13" s="33">
+        <v>130510</v>
+      </c>
+      <c r="S13" t="s">
         <v>602</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>611</v>
       </c>
-      <c r="S13" t="s">
+      <c r="U13" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
         <v>597</v>
       </c>
@@ -26304,14 +26809,16 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
       <c r="P14" s="30"/>
-      <c r="Q14" t="s">
+      <c r="Q14" s="30"/>
+      <c r="R14" s="33"/>
+      <c r="S14" t="s">
         <v>603</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
         <v>605</v>
       </c>
@@ -26344,8 +26851,10 @@
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
       <c r="P15" s="30"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q15" s="30"/>
+      <c r="R15" s="33"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>605</v>
       </c>
@@ -26378,8 +26887,10 @@
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
       <c r="P16" s="30"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q16" s="30"/>
+      <c r="R16" s="33"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>605</v>
       </c>
@@ -26412,8 +26923,10 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
       <c r="P17" s="30"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q17" s="30"/>
+      <c r="R17" s="33"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
         <v>605</v>
       </c>
@@ -26446,8 +26959,10 @@
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
       <c r="P18" s="30"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q18" s="30"/>
+      <c r="R18" s="33"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>605</v>
       </c>
@@ -26482,8 +26997,10 @@
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
       <c r="P19" s="30"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q19" s="30"/>
+      <c r="R19" s="33"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
         <v>605</v>
       </c>
@@ -26518,8 +27035,10 @@
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
       <c r="P20" s="30"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q20" s="30"/>
+      <c r="R20" s="33"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
         <v>605</v>
       </c>
@@ -26552,8 +27071,10 @@
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
       <c r="P21" s="30"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q21" s="30"/>
+      <c r="R21" s="33"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="33" t="s">
         <v>605</v>
       </c>
@@ -26588,8 +27109,10 @@
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
       <c r="P22" s="30"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q22" s="30"/>
+      <c r="R22" s="33"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="33" t="s">
         <v>605</v>
       </c>
@@ -26622,8 +27145,10 @@
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
       <c r="P23" s="30"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q23" s="30"/>
+      <c r="R23" s="33"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="33" t="s">
         <v>605</v>
       </c>
@@ -26658,8 +27183,10 @@
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
       <c r="P24" s="30"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q24" s="30"/>
+      <c r="R24" s="33"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="33" t="s">
         <v>605</v>
       </c>
@@ -26692,8 +27219,10 @@
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
       <c r="P25" s="30"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q25" s="30"/>
+      <c r="R25" s="33"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="33" t="s">
         <v>605</v>
       </c>
@@ -26726,8 +27255,10 @@
       <c r="N26" s="30"/>
       <c r="O26" s="30"/>
       <c r="P26" s="30"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q26" s="30"/>
+      <c r="R26" s="33"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
         <v>605</v>
       </c>
@@ -26760,8 +27291,10 @@
       <c r="N27" s="30"/>
       <c r="O27" s="30"/>
       <c r="P27" s="30"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q27" s="30"/>
+      <c r="R27" s="33"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="63" t="s">
         <v>598</v>
       </c>
@@ -26769,7 +27302,7 @@
         <v>131161</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D28" s="42">
         <v>2</v>
@@ -26782,7 +27315,7 @@
         <v>6</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I28" s="30"/>
       <c r="J28" s="30" t="s">
@@ -26796,8 +27329,10 @@
       <c r="N28" s="30"/>
       <c r="O28" s="30"/>
       <c r="P28" s="30"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q28" s="30"/>
+      <c r="R28" s="33"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>598</v>
       </c>
@@ -26832,8 +27367,10 @@
       <c r="N29" s="30"/>
       <c r="O29" s="30"/>
       <c r="P29" s="30"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q29" s="30"/>
+      <c r="R29" s="33"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="63" t="s">
         <v>598</v>
       </c>
@@ -26841,7 +27378,7 @@
         <v>131160</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D30" s="42">
         <v>4</v>
@@ -26854,7 +27391,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="I30" s="30"/>
       <c r="J30" s="30" t="s">
@@ -26868,8 +27405,10 @@
       <c r="N30" s="30"/>
       <c r="O30" s="30"/>
       <c r="P30" s="30"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q30" s="30"/>
+      <c r="R30" s="33"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="33" t="s">
         <v>598</v>
       </c>
@@ -26904,8 +27443,10 @@
       <c r="N31" s="30"/>
       <c r="O31" s="30"/>
       <c r="P31" s="30"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q31" s="30"/>
+      <c r="R31" s="33"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="63" t="s">
         <v>598</v>
       </c>
@@ -26913,7 +27454,7 @@
         <v>131149</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D32" s="42">
         <v>6</v>
@@ -26926,7 +27467,7 @@
         <v>6</v>
       </c>
       <c r="H32" s="42" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I32" s="30"/>
       <c r="J32" s="30" t="s">
@@ -26940,8 +27481,10 @@
       <c r="N32" s="30"/>
       <c r="O32" s="30"/>
       <c r="P32" s="30"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q32" s="30"/>
+      <c r="R32" s="33"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>598</v>
       </c>
@@ -26976,8 +27519,10 @@
       <c r="N33" s="30"/>
       <c r="O33" s="30"/>
       <c r="P33" s="30"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q33" s="30"/>
+      <c r="R33" s="33"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="63" t="s">
         <v>598</v>
       </c>
@@ -26985,7 +27530,7 @@
         <v>131148</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D34" s="42">
         <v>10</v>
@@ -26998,7 +27543,7 @@
         <v>6</v>
       </c>
       <c r="H34" s="42" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I34" s="39"/>
       <c r="J34" s="30" t="s">
@@ -27012,8 +27557,10 @@
       <c r="N34" s="30"/>
       <c r="O34" s="30"/>
       <c r="P34" s="30"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q34" s="30"/>
+      <c r="R34" s="33"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="33" t="s">
         <v>598</v>
       </c>
@@ -27048,8 +27595,10 @@
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
       <c r="P35" s="30"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q35" s="30"/>
+      <c r="R35" s="33"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="63" t="s">
         <v>598</v>
       </c>
@@ -27057,7 +27606,7 @@
         <v>131133</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D36" s="42">
         <v>6</v>
@@ -27070,7 +27619,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="42" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="I36" s="30"/>
       <c r="J36" s="30" t="s">
@@ -27084,8 +27633,10 @@
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
       <c r="P36" s="30"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q36" s="30"/>
+      <c r="R36" s="33"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="33" t="s">
         <v>598</v>
       </c>
@@ -27120,8 +27671,10 @@
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
       <c r="P37" s="30"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q37" s="30"/>
+      <c r="R37" s="33"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="33" t="s">
         <v>598</v>
       </c>
@@ -27156,8 +27709,10 @@
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
       <c r="P38" s="30"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q38" s="30"/>
+      <c r="R38" s="33"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="63" t="s">
         <v>598</v>
       </c>
@@ -27165,7 +27720,7 @@
         <v>131144</v>
       </c>
       <c r="C39" s="42" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D39" s="42">
         <v>6</v>
@@ -27178,7 +27733,7 @@
         <v>6</v>
       </c>
       <c r="H39" s="42" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="I39" s="30"/>
       <c r="J39" s="30" t="s">
@@ -27192,8 +27747,10 @@
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
       <c r="P39" s="30"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q39" s="30"/>
+      <c r="R39" s="33"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="33" t="s">
         <v>598</v>
       </c>
@@ -27228,8 +27785,10 @@
       <c r="N40" s="30"/>
       <c r="O40" s="30"/>
       <c r="P40" s="30"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q40" s="30"/>
+      <c r="R40" s="33"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="33" t="s">
         <v>598</v>
       </c>
@@ -27264,8 +27823,10 @@
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
       <c r="P41" s="30"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q41" s="30"/>
+      <c r="R41" s="33"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="63" t="s">
         <v>598</v>
       </c>
@@ -27273,7 +27834,7 @@
         <v>131145</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D42" s="42">
         <v>16</v>
@@ -27286,7 +27847,7 @@
         <v>10</v>
       </c>
       <c r="H42" s="42" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="I42" s="30"/>
       <c r="J42" s="30" t="s">
@@ -27300,8 +27861,10 @@
       <c r="N42" s="30"/>
       <c r="O42" s="30"/>
       <c r="P42" s="30"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q42" s="30"/>
+      <c r="R42" s="33"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="63" t="s">
         <v>598</v>
       </c>
@@ -27309,7 +27872,7 @@
         <v>131146</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="D43" s="42">
         <v>20</v>
@@ -27322,7 +27885,7 @@
         <v>10</v>
       </c>
       <c r="H43" s="42" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="I43" s="30"/>
       <c r="J43" s="30" t="s">
@@ -27336,8 +27899,10 @@
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
       <c r="P43" s="30"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q43" s="30"/>
+      <c r="R43" s="33"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
         <v>598</v>
       </c>
@@ -27372,8 +27937,10 @@
       <c r="N44" s="30"/>
       <c r="O44" s="30"/>
       <c r="P44" s="30"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q44" s="30"/>
+      <c r="R44" s="33"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
         <v>598</v>
       </c>
@@ -27408,8 +27975,10 @@
       <c r="N45" s="30"/>
       <c r="O45" s="30"/>
       <c r="P45" s="30"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q45" s="30"/>
+      <c r="R45" s="33"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
         <v>598</v>
       </c>
@@ -27444,8 +28013,10 @@
       <c r="N46" s="30"/>
       <c r="O46" s="30"/>
       <c r="P46" s="30"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q46" s="30"/>
+      <c r="R46" s="33"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
         <v>598</v>
       </c>
@@ -27480,8 +28051,10 @@
       <c r="N47" s="30"/>
       <c r="O47" s="30"/>
       <c r="P47" s="30"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q47" s="30"/>
+      <c r="R47" s="33"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="63" t="s">
         <v>598</v>
       </c>
@@ -27489,7 +28062,7 @@
         <v>131147</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D48" s="42">
         <v>50</v>
@@ -27502,7 +28075,7 @@
         <v>6</v>
       </c>
       <c r="H48" s="42" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I48" s="30"/>
       <c r="J48" s="30" t="s">
@@ -27516,8 +28089,10 @@
       <c r="N48" s="30"/>
       <c r="O48" s="30"/>
       <c r="P48" s="30"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q48" s="30"/>
+      <c r="R48" s="33"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
         <v>598</v>
       </c>
@@ -27552,8 +28127,10 @@
       <c r="N49" s="30"/>
       <c r="O49" s="30"/>
       <c r="P49" s="30"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q49" s="30"/>
+      <c r="R49" s="33"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="33" t="s">
         <v>598</v>
       </c>
@@ -27586,8 +28163,10 @@
       <c r="N50" s="30"/>
       <c r="O50" s="30"/>
       <c r="P50" s="30"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q50" s="30"/>
+      <c r="R50" s="33"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
         <v>598</v>
       </c>
@@ -27622,8 +28201,10 @@
       <c r="N51" s="30"/>
       <c r="O51" s="30"/>
       <c r="P51" s="30"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q51" s="30"/>
+      <c r="R51" s="33"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="33" t="s">
         <v>598</v>
       </c>
@@ -27658,8 +28239,10 @@
       <c r="N52" s="30"/>
       <c r="O52" s="30"/>
       <c r="P52" s="30"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q52" s="30"/>
+      <c r="R52" s="33"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="33" t="s">
         <v>598</v>
       </c>
@@ -27694,8 +28277,10 @@
       <c r="N53" s="30"/>
       <c r="O53" s="30"/>
       <c r="P53" s="30"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q53" s="30"/>
+      <c r="R53" s="33"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="33" t="s">
         <v>598</v>
       </c>
@@ -27730,8 +28315,10 @@
       <c r="N54" s="30"/>
       <c r="O54" s="30"/>
       <c r="P54" s="30"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q54" s="30"/>
+      <c r="R54" s="33"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="33" t="s">
         <v>598</v>
       </c>
@@ -27766,8 +28353,10 @@
       <c r="N55" s="30"/>
       <c r="O55" s="30"/>
       <c r="P55" s="30"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q55" s="30"/>
+      <c r="R55" s="33"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="33" t="s">
         <v>599</v>
       </c>
@@ -27802,8 +28391,10 @@
       <c r="N56" s="30"/>
       <c r="O56" s="30"/>
       <c r="P56" s="30"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q56" s="30"/>
+      <c r="R56" s="33"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="33" t="s">
         <v>599</v>
       </c>
@@ -27838,8 +28429,10 @@
       <c r="N57" s="30"/>
       <c r="O57" s="30"/>
       <c r="P57" s="30"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q57" s="30"/>
+      <c r="R57" s="33"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="33" t="s">
         <v>599</v>
       </c>
@@ -27874,8 +28467,10 @@
       <c r="N58" s="30"/>
       <c r="O58" s="30"/>
       <c r="P58" s="30"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q58" s="30"/>
+      <c r="R58" s="33"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="33" t="s">
         <v>599</v>
       </c>
@@ -27910,8 +28505,14 @@
       <c r="N59" s="30"/>
       <c r="O59" s="30"/>
       <c r="P59" s="30"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q59" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R59" s="33">
+        <v>130511</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="33" t="s">
         <v>599</v>
       </c>
@@ -27946,8 +28547,14 @@
       <c r="N60" s="30"/>
       <c r="O60" s="30"/>
       <c r="P60" s="30"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q60" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R60" s="33">
+        <v>130511</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="33" t="s">
         <v>599</v>
       </c>
@@ -27982,8 +28589,14 @@
       <c r="N61" s="30"/>
       <c r="O61" s="30"/>
       <c r="P61" s="30"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q61" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R61" s="33">
+        <v>130511</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="33" t="s">
         <v>599</v>
       </c>
@@ -28018,8 +28631,14 @@
       <c r="N62" s="30"/>
       <c r="O62" s="30"/>
       <c r="P62" s="30"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q62" s="30" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R62" s="33">
+        <v>130510</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="33" t="s">
         <v>599</v>
       </c>
@@ -28054,8 +28673,14 @@
       <c r="N63" s="30"/>
       <c r="O63" s="30"/>
       <c r="P63" s="30"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q63" s="30" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R63" s="33">
+        <v>130510</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="33" t="s">
         <v>599</v>
       </c>
@@ -28090,8 +28715,14 @@
       <c r="N64" s="30"/>
       <c r="O64" s="30"/>
       <c r="P64" s="30"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q64" s="30" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R64" s="33">
+        <v>130510</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="33" t="s">
         <v>599</v>
       </c>
@@ -28126,8 +28757,10 @@
       <c r="N65" s="30"/>
       <c r="O65" s="30"/>
       <c r="P65" s="30"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q65" s="30"/>
+      <c r="R65" s="33"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="33" t="s">
         <v>599</v>
       </c>
@@ -28162,8 +28795,10 @@
       <c r="N66" s="30"/>
       <c r="O66" s="30"/>
       <c r="P66" s="30"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q66" s="30"/>
+      <c r="R66" s="33"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="33" t="s">
         <v>599</v>
       </c>
@@ -28198,8 +28833,10 @@
       <c r="N67" s="30"/>
       <c r="O67" s="30"/>
       <c r="P67" s="30"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q67" s="30"/>
+      <c r="R67" s="33"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="33" t="s">
         <v>599</v>
       </c>
@@ -28234,8 +28871,10 @@
       <c r="N68" s="30"/>
       <c r="O68" s="30"/>
       <c r="P68" s="30"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q68" s="30"/>
+      <c r="R68" s="33"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="33" t="s">
         <v>599</v>
       </c>
@@ -28270,8 +28909,10 @@
       <c r="N69" s="30"/>
       <c r="O69" s="30"/>
       <c r="P69" s="30"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q69" s="30"/>
+      <c r="R69" s="33"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="33" t="s">
         <v>599</v>
       </c>
@@ -28304,8 +28945,10 @@
       <c r="N70" s="30"/>
       <c r="O70" s="30"/>
       <c r="P70" s="30"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q70" s="30"/>
+      <c r="R70" s="33"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="33" t="s">
         <v>600</v>
       </c>
@@ -28340,8 +28983,10 @@
         <v>0</v>
       </c>
       <c r="P71" s="30"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q71" s="30"/>
+      <c r="R71" s="33"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="33" t="s">
         <v>600</v>
       </c>
@@ -28376,8 +29021,10 @@
         <v>1</v>
       </c>
       <c r="P72" s="30"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q72" s="30"/>
+      <c r="R72" s="33"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="33" t="s">
         <v>600</v>
       </c>
@@ -28414,8 +29061,10 @@
       <c r="P73" s="30" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q73" s="30"/>
+      <c r="R73" s="33"/>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="33" t="s">
         <v>600</v>
       </c>
@@ -28452,8 +29101,10 @@
       <c r="P74" s="30" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q74" s="30"/>
+      <c r="R74" s="33"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="33" t="s">
         <v>600</v>
       </c>
@@ -28490,8 +29141,10 @@
       <c r="P75" s="30" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q75" s="30"/>
+      <c r="R75" s="33"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="33" t="s">
         <v>600</v>
       </c>
@@ -28530,8 +29183,10 @@
       <c r="P76" s="30" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q76" s="30"/>
+      <c r="R76" s="33"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
         <v>601</v>
       </c>
@@ -28568,8 +29223,10 @@
       <c r="P77" s="30" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q77" s="30"/>
+      <c r="R77" s="33"/>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
         <v>601</v>
       </c>
@@ -28606,8 +29263,10 @@
       <c r="P78" s="30">
         <v>220</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q78" s="30"/>
+      <c r="R78" s="33"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
         <v>601</v>
       </c>
@@ -28644,8 +29303,10 @@
       <c r="P79" s="30">
         <v>220</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q79" s="30"/>
+      <c r="R79" s="33"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
         <v>601</v>
       </c>
@@ -28682,8 +29343,10 @@
       <c r="P80" s="30">
         <v>220</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q80" s="30"/>
+      <c r="R80" s="33"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="33" t="s">
         <v>809</v>
       </c>
@@ -28718,8 +29381,10 @@
         <v>0</v>
       </c>
       <c r="P81" s="30"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q81" s="30"/>
+      <c r="R81" s="33"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="33" t="s">
         <v>602</v>
       </c>
@@ -28752,8 +29417,10 @@
       <c r="N82" s="30"/>
       <c r="O82" s="30"/>
       <c r="P82" s="30"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q82" s="30"/>
+      <c r="R82" s="33"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="33" t="s">
         <v>603</v>
       </c>
@@ -28782,6 +29449,8 @@
       <c r="N83" s="30"/>
       <c r="O83" s="30"/>
       <c r="P83" s="30"/>
+      <c r="Q83" s="30"/>
+      <c r="R83" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -56705,7 +57374,7 @@
         <v>1111</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D79" s="30"/>
       <c r="E79" s="30">
@@ -56767,14 +57436,14 @@
         <v>132192</v>
       </c>
       <c r="C81" s="30" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D81" s="30"/>
       <c r="E81" s="30"/>
       <c r="F81" s="30"/>
       <c r="G81" s="30"/>
       <c r="H81" s="30" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I81" s="30"/>
       <c r="J81" s="30"/>
@@ -56794,14 +57463,14 @@
         <v>131107</v>
       </c>
       <c r="C82" s="30" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30"/>
       <c r="F82" s="30"/>
       <c r="G82" s="30"/>
       <c r="H82" s="30" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="I82" s="30"/>
       <c r="J82" s="30"/>
@@ -56821,7 +57490,7 @@
         <v>130993</v>
       </c>
       <c r="C83" s="30" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D83" s="30"/>
       <c r="E83" s="30" t="s">
@@ -56830,7 +57499,7 @@
       <c r="F83" s="30"/>
       <c r="G83" s="30"/>
       <c r="H83" s="33" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I83" s="30"/>
       <c r="J83" s="30"/>
@@ -56854,7 +57523,7 @@
         <v>130384</v>
       </c>
       <c r="C84" s="30" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D84" s="30"/>
       <c r="E84" s="30" t="s">
@@ -56863,7 +57532,7 @@
       <c r="F84" s="30"/>
       <c r="G84" s="30"/>
       <c r="H84" s="33" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I84" s="30"/>
       <c r="J84" s="30"/>
@@ -56887,7 +57556,7 @@
         <v>130383</v>
       </c>
       <c r="C85" s="30" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D85" s="30"/>
       <c r="E85" s="30" t="s">
@@ -56896,7 +57565,7 @@
       <c r="F85" s="30"/>
       <c r="G85" s="30"/>
       <c r="H85" s="33" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I85" s="30"/>
       <c r="J85" s="30"/>
@@ -56951,7 +57620,7 @@
         <v>130994</v>
       </c>
       <c r="C87" s="30" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D87" s="30"/>
       <c r="E87" s="30" t="s">
@@ -56960,7 +57629,7 @@
       <c r="F87" s="30"/>
       <c r="G87" s="30"/>
       <c r="H87" s="33" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="I87" s="30"/>
       <c r="J87" s="30"/>
@@ -56984,7 +57653,7 @@
         <v>130271</v>
       </c>
       <c r="C88" s="30" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D88" s="30"/>
       <c r="E88" s="30" t="s">
@@ -56993,7 +57662,7 @@
       <c r="F88" s="30"/>
       <c r="G88" s="30"/>
       <c r="H88" s="33" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="I88" s="30"/>
       <c r="J88" s="30"/>
@@ -57017,14 +57686,14 @@
         <v>132085</v>
       </c>
       <c r="C89" s="33" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D89" s="30"/>
       <c r="E89" s="30"/>
       <c r="F89" s="30"/>
       <c r="G89" s="30"/>
       <c r="H89" s="33" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I89" s="30"/>
       <c r="J89" s="30"/>
@@ -57044,14 +57713,14 @@
         <v>131004</v>
       </c>
       <c r="C90" s="30" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="30"/>
       <c r="F90" s="30"/>
       <c r="G90" s="30"/>
       <c r="H90" s="30" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I90" s="30"/>
       <c r="J90" s="30"/>
@@ -57096,14 +57765,14 @@
         <v>130058</v>
       </c>
       <c r="C92" s="30" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="30"/>
       <c r="F92" s="30"/>
       <c r="G92" s="30"/>
       <c r="H92" s="30" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I92" s="30"/>
       <c r="J92" s="30"/>
@@ -57123,14 +57792,14 @@
         <v>130182</v>
       </c>
       <c r="C93" s="30" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D93" s="30"/>
       <c r="E93" s="30"/>
       <c r="F93" s="30"/>
       <c r="G93" s="30"/>
       <c r="H93" s="30" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I93" s="30"/>
       <c r="J93" s="30"/>
@@ -57150,7 +57819,7 @@
         <v>139604</v>
       </c>
       <c r="C94" s="30" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D94" s="30"/>
       <c r="E94" s="30"/>
@@ -57177,7 +57846,7 @@
         <v>130077</v>
       </c>
       <c r="C95" s="30" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D95" s="30"/>
       <c r="E95" s="30"/>
@@ -57198,20 +57867,20 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="33" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B96" s="30">
         <v>130389</v>
       </c>
       <c r="C96" s="33" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D96" s="30"/>
       <c r="E96" s="30"/>
       <c r="F96" s="30"/>
       <c r="G96" s="30"/>
       <c r="H96" s="33" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="I96" s="30"/>
       <c r="J96" s="30"/>
@@ -57230,16 +57899,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7C9F8C-4259-48F2-9724-29D595F3E5AD}">
-  <dimension ref="A1:S93"/>
+  <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B70" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView topLeftCell="G66" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -60257,170 +60926,450 @@
       <c r="P82" s="30"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A83" s="52" t="s">
+      <c r="A83" s="33" t="s">
         <v>819</v>
       </c>
-      <c r="C83" s="52" t="s">
+      <c r="B83" s="33"/>
+      <c r="C83" s="33" t="s">
         <v>871</v>
       </c>
-      <c r="E83" t="s">
+      <c r="D83" s="33"/>
+      <c r="E83" s="33" t="s">
         <v>821</v>
       </c>
-      <c r="H83" s="52" t="s">
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="30" t="s">
         <v>820</v>
       </c>
-      <c r="P83">
+      <c r="I83" s="33"/>
+      <c r="J83" s="33"/>
+      <c r="K83" s="33"/>
+      <c r="L83" s="33"/>
+      <c r="M83" s="33"/>
+      <c r="N83" s="33"/>
+      <c r="O83" s="33"/>
+      <c r="P83" s="33">
         <v>220</v>
       </c>
-      <c r="Q83">
+      <c r="Q83" s="33">
         <v>460</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A84" s="52" t="s">
+      <c r="A84" s="33" t="s">
         <v>819</v>
       </c>
-      <c r="C84" s="52" t="s">
+      <c r="B84" s="33"/>
+      <c r="C84" s="33" t="s">
         <v>871</v>
       </c>
-      <c r="E84" t="s">
+      <c r="D84" s="33"/>
+      <c r="E84" s="33" t="s">
         <v>859</v>
       </c>
-      <c r="H84" s="52" t="s">
+      <c r="F84" s="33"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="30" t="s">
         <v>820</v>
       </c>
-      <c r="P84">
+      <c r="I84" s="33"/>
+      <c r="J84" s="33"/>
+      <c r="K84" s="33"/>
+      <c r="L84" s="33"/>
+      <c r="M84" s="33"/>
+      <c r="N84" s="33"/>
+      <c r="O84" s="33"/>
+      <c r="P84" s="33">
         <v>220</v>
       </c>
-      <c r="Q84">
+      <c r="Q84" s="33">
         <v>460</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A85" s="52" t="s">
+      <c r="A85" s="33" t="s">
         <v>810</v>
       </c>
-      <c r="C85" s="52" t="s">
+      <c r="B85" s="33"/>
+      <c r="C85" s="33" t="s">
         <v>872</v>
       </c>
-      <c r="H85" s="52" t="s">
+      <c r="D85" s="33"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="33"/>
+      <c r="H85" s="30" t="s">
         <v>825</v>
       </c>
+      <c r="I85" s="33"/>
+      <c r="J85" s="33"/>
+      <c r="K85" s="33"/>
+      <c r="L85" s="33"/>
+      <c r="M85" s="33"/>
+      <c r="N85" s="33"/>
+      <c r="O85" s="33"/>
+      <c r="P85" s="33"/>
+      <c r="Q85" s="33"/>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A86" s="52" t="s">
+      <c r="A86" s="33" t="s">
         <v>827</v>
       </c>
-      <c r="C86" s="52" t="s">
+      <c r="B86" s="33"/>
+      <c r="C86" s="33" t="s">
         <v>873</v>
       </c>
-      <c r="H86" s="52" t="s">
+      <c r="D86" s="33"/>
+      <c r="E86" s="33"/>
+      <c r="F86" s="33"/>
+      <c r="G86" s="33"/>
+      <c r="H86" s="30" t="s">
         <v>828</v>
       </c>
+      <c r="I86" s="33"/>
+      <c r="J86" s="33"/>
+      <c r="K86" s="33"/>
+      <c r="L86" s="33"/>
+      <c r="M86" s="33"/>
+      <c r="N86" s="33"/>
+      <c r="O86" s="33"/>
+      <c r="P86" s="33"/>
+      <c r="Q86" s="33"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A87" s="52" t="s">
+      <c r="A87" s="33" t="s">
         <v>811</v>
       </c>
-      <c r="C87" s="52" t="s">
+      <c r="B87" s="33"/>
+      <c r="C87" s="33" t="s">
         <v>877</v>
       </c>
-      <c r="H87" s="52" t="s">
+      <c r="D87" s="33"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="33"/>
+      <c r="G87" s="33"/>
+      <c r="H87" s="30" t="s">
         <v>833</v>
       </c>
+      <c r="I87" s="33"/>
+      <c r="J87" s="33"/>
+      <c r="K87" s="33"/>
+      <c r="L87" s="33"/>
+      <c r="M87" s="33"/>
+      <c r="N87" s="33"/>
+      <c r="O87" s="33"/>
+      <c r="P87" s="33"/>
+      <c r="Q87" s="33"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A88" s="52" t="s">
+      <c r="A88" s="33" t="s">
         <v>812</v>
       </c>
-      <c r="C88" s="52" t="s">
+      <c r="B88" s="33"/>
+      <c r="C88" s="33" t="s">
         <v>880</v>
       </c>
-      <c r="H88" s="52" t="s">
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="30" t="s">
         <v>834</v>
       </c>
+      <c r="I88" s="33"/>
+      <c r="J88" s="33"/>
+      <c r="K88" s="33"/>
+      <c r="L88" s="33"/>
+      <c r="M88" s="33"/>
+      <c r="N88" s="33"/>
+      <c r="O88" s="33"/>
+      <c r="P88" s="33"/>
+      <c r="Q88" s="33"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A89" s="52" t="s">
+      <c r="A89" s="33" t="s">
         <v>813</v>
       </c>
-      <c r="C89" s="52" t="s">
+      <c r="B89" s="33"/>
+      <c r="C89" s="33" t="s">
         <v>843</v>
       </c>
-      <c r="H89" s="52" t="s">
+      <c r="D89" s="33"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
+      <c r="G89" s="33"/>
+      <c r="H89" s="30" t="s">
         <v>843</v>
       </c>
+      <c r="I89" s="33"/>
+      <c r="J89" s="33"/>
+      <c r="K89" s="33"/>
+      <c r="L89" s="33"/>
+      <c r="M89" s="33"/>
+      <c r="N89" s="33"/>
+      <c r="O89" s="33"/>
+      <c r="P89" s="33"/>
+      <c r="Q89" s="33"/>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A90" s="52" t="s">
+      <c r="A90" s="33" t="s">
         <v>844</v>
       </c>
-      <c r="C90" s="52" t="s">
+      <c r="B90" s="33"/>
+      <c r="C90" s="33" t="s">
         <v>621</v>
       </c>
-      <c r="H90" s="52" t="s">
+      <c r="D90" s="33"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="33"/>
+      <c r="G90" s="33"/>
+      <c r="H90" s="30" t="s">
         <v>621</v>
       </c>
+      <c r="I90" s="33"/>
+      <c r="J90" s="33"/>
+      <c r="K90" s="33"/>
+      <c r="L90" s="33"/>
+      <c r="M90" s="33"/>
+      <c r="N90" s="33"/>
+      <c r="O90" s="33"/>
+      <c r="P90" s="33"/>
+      <c r="Q90" s="33"/>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A91" s="52" t="s">
-        <v>1041</v>
+      <c r="A91" s="33" t="s">
+        <v>1040</v>
       </c>
       <c r="B91" s="33">
         <v>130244</v>
       </c>
-      <c r="C91" s="52" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D91">
+      <c r="C91" s="33" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D91" s="33">
         <v>65</v>
       </c>
-      <c r="H91" s="52" t="s">
-        <v>1045</v>
-      </c>
-      <c r="J91" t="s">
+      <c r="E91" s="33"/>
+      <c r="F91" s="33"/>
+      <c r="G91" s="33"/>
+      <c r="H91" s="30" t="s">
+        <v>1044</v>
+      </c>
+      <c r="I91" s="33"/>
+      <c r="J91" s="30" t="s">
         <v>44</v>
       </c>
+      <c r="K91" s="33"/>
+      <c r="L91" s="33"/>
+      <c r="M91" s="33"/>
+      <c r="N91" s="33"/>
+      <c r="O91" s="33"/>
+      <c r="P91" s="33"/>
+      <c r="Q91" s="33"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A92" s="52" t="s">
-        <v>1041</v>
+      <c r="A92" s="33" t="s">
+        <v>1040</v>
       </c>
       <c r="B92" s="33">
         <v>130247</v>
       </c>
-      <c r="C92" s="52" t="s">
-        <v>1043</v>
-      </c>
-      <c r="D92">
+      <c r="C92" s="33" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D92" s="33">
         <v>125</v>
       </c>
-      <c r="H92" s="52" t="s">
-        <v>1042</v>
-      </c>
-      <c r="J92" t="s">
+      <c r="E92" s="33"/>
+      <c r="F92" s="33"/>
+      <c r="G92" s="33"/>
+      <c r="H92" s="30" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I92" s="33"/>
+      <c r="J92" s="30" t="s">
         <v>443</v>
       </c>
+      <c r="K92" s="33"/>
+      <c r="L92" s="33"/>
+      <c r="M92" s="33"/>
+      <c r="N92" s="33"/>
+      <c r="O92" s="33"/>
+      <c r="P92" s="33"/>
+      <c r="Q92" s="33"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A93" s="52" t="s">
-        <v>1041</v>
+      <c r="A93" s="33" t="s">
+        <v>1040</v>
       </c>
       <c r="B93" s="33">
         <v>130240</v>
       </c>
-      <c r="C93" s="52" t="s">
-        <v>1048</v>
-      </c>
-      <c r="D93">
+      <c r="C93" s="33" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D93" s="33">
         <v>160</v>
       </c>
-      <c r="H93" s="52" t="s">
-        <v>1047</v>
-      </c>
-      <c r="J93" t="s">
+      <c r="E93" s="33"/>
+      <c r="F93" s="33"/>
+      <c r="G93" s="33"/>
+      <c r="H93" s="30" t="s">
+        <v>1046</v>
+      </c>
+      <c r="I93" s="33"/>
+      <c r="J93" s="30" t="s">
         <v>44</v>
       </c>
+      <c r="K93" s="33"/>
+      <c r="L93" s="33"/>
+      <c r="M93" s="33"/>
+      <c r="N93" s="33"/>
+      <c r="O93" s="33"/>
+      <c r="P93" s="33"/>
+      <c r="Q93" s="33"/>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A94" s="33" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B94" s="33">
+        <v>130232</v>
+      </c>
+      <c r="C94" s="33" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D94" s="33"/>
+      <c r="E94" s="33"/>
+      <c r="F94" s="33"/>
+      <c r="G94" s="33"/>
+      <c r="H94" s="30" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I94" s="33"/>
+      <c r="J94" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="K94" s="33"/>
+      <c r="L94" s="33"/>
+      <c r="M94" s="33"/>
+      <c r="N94" s="33"/>
+      <c r="O94" s="33"/>
+      <c r="P94" s="33"/>
+      <c r="Q94" s="33"/>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A95" s="33" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B95" s="33">
+        <v>130234</v>
+      </c>
+      <c r="C95" s="33" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D95" s="33"/>
+      <c r="E95" s="33"/>
+      <c r="F95" s="33"/>
+      <c r="G95" s="33"/>
+      <c r="H95" s="30" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I95" s="33"/>
+      <c r="J95" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="K95" s="33"/>
+      <c r="L95" s="33"/>
+      <c r="M95" s="33"/>
+      <c r="N95" s="33"/>
+      <c r="O95" s="33"/>
+      <c r="P95" s="33"/>
+      <c r="Q95" s="33"/>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A96" s="33" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B96" s="33">
+        <v>130233</v>
+      </c>
+      <c r="C96" s="33" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33"/>
+      <c r="G96" s="33"/>
+      <c r="H96" s="30" t="s">
+        <v>1076</v>
+      </c>
+      <c r="I96" s="33"/>
+      <c r="J96" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="K96" s="33"/>
+      <c r="L96" s="33"/>
+      <c r="M96" s="33"/>
+      <c r="N96" s="33"/>
+      <c r="O96" s="33"/>
+      <c r="P96" s="33"/>
+      <c r="Q96" s="33"/>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A97" s="33" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B97" s="33">
+        <v>130220</v>
+      </c>
+      <c r="C97" s="33" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D97" s="33"/>
+      <c r="E97" s="33"/>
+      <c r="F97" s="33"/>
+      <c r="G97" s="33"/>
+      <c r="H97" s="30" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I97" s="33"/>
+      <c r="J97" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="K97" s="33"/>
+      <c r="L97" s="33"/>
+      <c r="M97" s="33"/>
+      <c r="N97" s="33"/>
+      <c r="O97" s="33"/>
+      <c r="P97" s="33"/>
+      <c r="Q97" s="33"/>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A98" s="33" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B98" s="33">
+        <v>130243</v>
+      </c>
+      <c r="C98" s="33" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D98" s="33"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="33"/>
+      <c r="G98" s="33"/>
+      <c r="H98" s="30" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I98" s="33"/>
+      <c r="J98" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="K98" s="33"/>
+      <c r="L98" s="33"/>
+      <c r="M98" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -63604,27 +64553,27 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="33" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B96" s="30"/>
       <c r="C96" s="33" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D96" s="30"/>
       <c r="E96" s="30"/>
       <c r="F96" s="30"/>
       <c r="G96" s="30"/>
       <c r="H96" s="33" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="33" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B97" s="30"/>
       <c r="C97" s="33" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D97" s="30"/>
       <c r="E97" s="30">
@@ -63633,16 +64582,16 @@
       <c r="F97" s="30"/>
       <c r="G97" s="30"/>
       <c r="H97" s="33" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="33" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B98" s="30"/>
       <c r="C98" s="33" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D98" s="30"/>
       <c r="E98" s="30">
@@ -63651,7 +64600,7 @@
       <c r="F98" s="30"/>
       <c r="G98" s="30"/>
       <c r="H98" s="33" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>